<commit_message>
Changed schedule practical descriptions
</commit_message>
<xml_diff>
--- a/BB512_Schedule.xlsx
+++ b/BB512_Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jones/Dropbox/_SDU_Teaching/BB512/Course Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF157941-FF31-A143-92D9-FB72C9A38A6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FBD3A3-3276-9440-95AC-A58EE7DD9764}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="27220" xr2:uid="{CCA45BD5-8A90-4848-8BF8-FC958BC91D48}"/>
   </bookViews>
@@ -77,9 +77,6 @@
     <t>TBB</t>
   </si>
   <si>
-    <t>Excel exercises on exponential/geometric growth</t>
-  </si>
-  <si>
     <t>Extra reading</t>
   </si>
   <si>
@@ -92,24 +89,15 @@
     <t>Logistic growth 1</t>
   </si>
   <si>
-    <t>Excel exercises on logistic growth</t>
-  </si>
-  <si>
     <t>G.2</t>
   </si>
   <si>
     <t>Logistic growth 2</t>
   </si>
   <si>
-    <t>Excel, deeper into logistic growth, different perspectives</t>
-  </si>
-  <si>
     <t>Age &amp; stage structured models</t>
   </si>
   <si>
-    <t>Excel, life tables</t>
-  </si>
-  <si>
     <t>G.3</t>
   </si>
   <si>
@@ -119,21 +107,12 @@
     <t>Predation 1</t>
   </si>
   <si>
-    <t>Exercises on matrix models</t>
-  </si>
-  <si>
     <t>G.6</t>
   </si>
   <si>
     <t>Exercises on predation</t>
   </si>
   <si>
-    <t>Lemming case study 1</t>
-  </si>
-  <si>
-    <t>Lemming case study 2</t>
-  </si>
-  <si>
     <t> Berg et al. (2008) High-Arctic Plant–Herbivore Interactions under Climate Influence. Advances in Arctic Research. 40: 275-298; Schmidt et al (2008) Vertebrate Predator-Prey Interactions in a Seasonal Environment. 40: 345-370.</t>
   </si>
   <si>
@@ -257,9 +236,6 @@
     <t>Exponential growth 2</t>
   </si>
   <si>
-    <t>Excel exercises on stochastic exponential growth</t>
-  </si>
-  <si>
     <t>Competition 1</t>
   </si>
   <si>
@@ -270,6 +246,30 @@
   </si>
   <si>
     <t>Population Biology</t>
+  </si>
+  <si>
+    <t>Matrix population modeling</t>
+  </si>
+  <si>
+    <t>Legend of Ambalapuzha; Geometric growth</t>
+  </si>
+  <si>
+    <t>Stochastic population growth</t>
+  </si>
+  <si>
+    <t>Basic logistic population growth</t>
+  </si>
+  <si>
+    <t>Deeper into logistic growth</t>
+  </si>
+  <si>
+    <t>Life tables</t>
+  </si>
+  <si>
+    <t>Lemming case study part 1</t>
+  </si>
+  <si>
+    <t>Lemming case study part 2</t>
   </si>
 </sst>
 </file>
@@ -632,7 +632,7 @@
   <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B21"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -661,7 +661,7 @@
         <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -669,7 +669,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -681,7 +681,7 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>10</v>
@@ -692,7 +692,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -709,7 +709,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -721,7 +721,7 @@
         <v>13</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -729,19 +729,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -749,19 +749,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -769,19 +769,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E7" t="s">
         <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -789,19 +789,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
         <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -809,19 +809,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>19</v>
+        <v>74</v>
       </c>
       <c r="E9" t="s">
         <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -829,19 +829,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E10" t="s">
         <v>13</v>
       </c>
       <c r="F10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -849,19 +849,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="E11" t="s">
         <v>8</v>
       </c>
       <c r="F11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -869,19 +869,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E12" t="s">
         <v>8</v>
       </c>
       <c r="F12" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -889,19 +889,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C13" t="s">
         <v>1</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>24</v>
+        <v>76</v>
       </c>
       <c r="E13" t="s">
         <v>8</v>
       </c>
       <c r="F13" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -909,19 +909,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="E14" t="s">
         <v>13</v>
       </c>
       <c r="F14" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -929,19 +929,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="E15" t="s">
         <v>13</v>
       </c>
       <c r="F15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -949,19 +949,19 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E16" t="s">
         <v>13</v>
       </c>
       <c r="F16" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -969,19 +969,19 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C17" t="s">
         <v>1</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="E17" t="s">
         <v>8</v>
       </c>
       <c r="F17" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -989,19 +989,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C18" t="s">
         <v>2</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="E18" t="s">
         <v>13</v>
       </c>
       <c r="F18" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1009,19 +1009,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C19" t="s">
         <v>1</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E19" t="s">
         <v>8</v>
       </c>
       <c r="F19" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1029,19 +1029,19 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>31</v>
+        <v>77</v>
       </c>
       <c r="E20" t="s">
         <v>13</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1049,13 +1049,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="C21" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="E21" t="s">
         <v>13</v>
@@ -1066,19 +1066,19 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C22" t="s">
         <v>2</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E22" t="s">
         <v>8</v>
       </c>
       <c r="F22" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1086,19 +1086,19 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C23" t="s">
         <v>1</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E23" t="s">
         <v>8</v>
       </c>
       <c r="F23" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1106,19 +1106,19 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C24" t="s">
         <v>2</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E24" t="s">
         <v>8</v>
       </c>
       <c r="F24" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1126,19 +1126,19 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C25" t="s">
         <v>1</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E25" t="s">
         <v>8</v>
       </c>
       <c r="F25" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1146,22 +1146,22 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C26" t="s">
         <v>2</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E26" t="s">
         <v>8</v>
       </c>
       <c r="F26" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1169,19 +1169,19 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C27" t="s">
-        <v>1</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="E27" t="s">
         <v>8</v>
       </c>
       <c r="F27" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1189,19 +1189,19 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C28" t="s">
         <v>2</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E28" t="s">
         <v>8</v>
       </c>
       <c r="F28" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1209,13 +1209,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C29" t="s">
         <v>1</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E29" t="s">
         <v>8</v>
@@ -1226,19 +1226,19 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C30" t="s">
         <v>2</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E30" t="s">
         <v>8</v>
       </c>
       <c r="F30" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1246,13 +1246,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C31" t="s">
         <v>1</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E31" t="s">
         <v>8</v>
@@ -1263,19 +1263,19 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C32" t="s">
         <v>2</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E32" t="s">
         <v>8</v>
       </c>
       <c r="F32" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1283,13 +1283,13 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C33" t="s">
         <v>1</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E33" t="s">
         <v>8</v>
@@ -1300,22 +1300,22 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C34" t="s">
         <v>2</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E34" t="s">
         <v>8</v>
       </c>
       <c r="F34" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1323,19 +1323,19 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C35" t="s">
         <v>1</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E35" t="s">
         <v>8</v>
       </c>
       <c r="F35" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1343,22 +1343,22 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C36" t="s">
         <v>2</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E36" t="s">
         <v>8</v>
       </c>
       <c r="F36" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1366,13 +1366,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C37" t="s">
         <v>1</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E37" t="s">
         <v>8</v>
@@ -1383,19 +1383,19 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C38" t="s">
         <v>2</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E38" t="s">
         <v>8</v>
       </c>
       <c r="F38" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1403,13 +1403,13 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C39" t="s">
         <v>1</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E39" t="s">
         <v>8</v>
@@ -1420,22 +1420,22 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C40" t="s">
         <v>2</v>
       </c>
       <c r="D40" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E40" t="s">
+        <v>8</v>
+      </c>
+      <c r="F40" t="s">
+        <v>58</v>
+      </c>
+      <c r="G40" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="E40" t="s">
-        <v>8</v>
-      </c>
-      <c r="F40" t="s">
-        <v>65</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1443,13 +1443,13 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C41" t="s">
         <v>1</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E41" t="s">
         <v>8</v>
@@ -1460,19 +1460,19 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C42" t="s">
         <v>2</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E42" t="s">
         <v>8</v>
       </c>
       <c r="F42" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1480,13 +1480,13 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C43" t="s">
         <v>1</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E43" t="s">
         <v>8</v>
@@ -1497,19 +1497,19 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C44" t="s">
         <v>2</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="E44" t="s">
         <v>8</v>
       </c>
       <c r="F44" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -1517,13 +1517,13 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C45" t="s">
         <v>1</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E45" t="s">
         <v>8</v>
@@ -1534,7 +1534,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C46" t="s">
         <v>2</v>
@@ -1548,7 +1548,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C47" t="s">
         <v>1</v>
@@ -1562,7 +1562,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C48" t="s">
         <v>2</v>
@@ -1576,7 +1576,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C49" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
Added JJ to the schedule
</commit_message>
<xml_diff>
--- a/BB512_Schedule.xlsx
+++ b/BB512_Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jones/Dropbox/_SDU_Teaching/BB512/Course Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0445647-C2E4-5A41-ADBE-3837DAB64426}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE95249-D393-B549-AE4C-3848BC453098}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="27220" xr2:uid="{CCA45BD5-8A90-4848-8BF8-FC958BC91D48}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="81">
   <si>
     <t>Topic</t>
   </si>
@@ -273,6 +273,9 @@
   </si>
   <si>
     <t>Lotka-Volterra competition</t>
+  </si>
+  <si>
+    <t>JJ</t>
   </si>
 </sst>
 </file>
@@ -643,7 +646,7 @@
   <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -909,7 +912,7 @@
         <v>73</v>
       </c>
       <c r="E13" t="s">
-        <v>8</v>
+        <v>80</v>
       </c>
       <c r="F13" t="s">
         <v>20</v>
@@ -929,7 +932,7 @@
         <v>63</v>
       </c>
       <c r="E14" t="s">
-        <v>8</v>
+        <v>80</v>
       </c>
       <c r="F14" t="s">
         <v>20</v>
@@ -949,7 +952,7 @@
         <v>63</v>
       </c>
       <c r="E15" t="s">
-        <v>8</v>
+        <v>80</v>
       </c>
       <c r="F15" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Added JJ to lecture
</commit_message>
<xml_diff>
--- a/BB512_Schedule.xlsx
+++ b/BB512_Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jones/Dropbox/_SDU_Teaching/BB512/Course Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE95249-D393-B549-AE4C-3848BC453098}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C0FBA65-7AD6-7847-BEFE-BFF0944A0101}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="27220" xr2:uid="{CCA45BD5-8A90-4848-8BF8-FC958BC91D48}"/>
   </bookViews>
@@ -646,7 +646,7 @@
   <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -892,7 +892,7 @@
         <v>19</v>
       </c>
       <c r="E12" t="s">
-        <v>8</v>
+        <v>80</v>
       </c>
       <c r="F12" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Rebuild with updated schedule
</commit_message>
<xml_diff>
--- a/BB512_Schedule.xlsx
+++ b/BB512_Schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jones/Dropbox/_SDU_Teaching/BB512/Course Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C0FBA65-7AD6-7847-BEFE-BFF0944A0101}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91516EA8-25BB-6C47-B480-5DD8405883A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="27220" xr2:uid="{CCA45BD5-8A90-4848-8BF8-FC958BC91D48}"/>
   </bookViews>
@@ -282,7 +282,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -646,16 +646,16 @@
   <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="48" style="1" customWidth="1"/>
     <col min="5" max="5" width="17.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -678,7 +678,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -701,7 +701,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -718,7 +718,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -738,7 +738,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -758,7 +758,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -778,7 +778,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -798,7 +798,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -818,7 +818,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -838,7 +838,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -858,7 +858,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -878,7 +878,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -898,7 +898,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -918,7 +918,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -938,7 +938,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -958,7 +958,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -978,7 +978,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -998,7 +998,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1038,7 +1038,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1061,7 +1061,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1081,12 +1081,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="C22" t="s">
         <v>2</v>
@@ -1098,12 +1098,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="C23" t="s">
         <v>2</v>
@@ -1115,7 +1115,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1135,7 +1135,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1155,7 +1155,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1238,7 +1238,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1258,7 +1258,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1275,7 +1275,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1472,7 +1472,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1529,7 +1529,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1546,7 +1546,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1583,7 +1583,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1595,7 +1595,7 @@
       </c>
       <c r="E48"/>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>

</xml_diff>

<commit_message>
Added practical: from population biology to fitness
</commit_message>
<xml_diff>
--- a/BB512_Schedule.xlsx
+++ b/BB512_Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jones/Dropbox/_SDU_Teaching/BB512/Course Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91516EA8-25BB-6C47-B480-5DD8405883A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B42CD1D-B841-9F4E-873D-8D3C5E425237}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="27220" xr2:uid="{CCA45BD5-8A90-4848-8BF8-FC958BC91D48}"/>
   </bookViews>
@@ -113,9 +113,6 @@
     <t>Evolution</t>
   </si>
   <si>
-    <t>Linking pop bio to evolution</t>
-  </si>
-  <si>
     <t>SH.1 &amp; appendix</t>
   </si>
   <si>
@@ -276,6 +273,9 @@
   </si>
   <si>
     <t>JJ</t>
+  </si>
+  <si>
+    <t>From population biology to fitness</t>
   </si>
 </sst>
 </file>
@@ -646,7 +646,7 @@
   <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -683,13 +683,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -706,7 +706,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -723,7 +723,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -743,13 +743,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
@@ -763,13 +763,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>12</v>
@@ -783,13 +783,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E7" t="s">
         <v>8</v>
@@ -803,7 +803,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -823,13 +823,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E9" t="s">
         <v>8</v>
@@ -843,7 +843,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
@@ -863,13 +863,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E11" t="s">
         <v>8</v>
@@ -883,7 +883,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -892,7 +892,7 @@
         <v>19</v>
       </c>
       <c r="E12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F12" t="s">
         <v>20</v>
@@ -903,16 +903,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C13" t="s">
         <v>1</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F13" t="s">
         <v>20</v>
@@ -923,16 +923,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="E14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F14" t="s">
         <v>20</v>
@@ -943,16 +943,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="E15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F15" t="s">
         <v>20</v>
@@ -963,13 +963,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E16" t="s">
         <v>12</v>
@@ -983,13 +983,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E17" t="s">
         <v>12</v>
@@ -1003,7 +1003,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C18" t="s">
         <v>2</v>
@@ -1023,13 +1023,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C19" t="s">
         <v>1</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E19" t="s">
         <v>8</v>
@@ -1043,13 +1043,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E20" t="s">
         <v>12</v>
@@ -1066,13 +1066,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C21" t="s">
         <v>1</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E21" t="s">
         <v>8</v>
@@ -1086,13 +1086,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C22" t="s">
         <v>2</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E22" t="s">
         <v>12</v>
@@ -1103,13 +1103,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C23" t="s">
         <v>2</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E23" t="s">
         <v>12</v>
@@ -1126,13 +1126,13 @@
         <v>2</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E24" t="s">
         <v>8</v>
       </c>
       <c r="F24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -1146,13 +1146,13 @@
         <v>1</v>
       </c>
       <c r="D25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E25" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" t="s">
         <v>26</v>
-      </c>
-      <c r="E25" t="s">
-        <v>8</v>
-      </c>
-      <c r="F25" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -1166,16 +1166,16 @@
         <v>2</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E26" t="s">
         <v>8</v>
       </c>
       <c r="F26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -1189,13 +1189,13 @@
         <v>1</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E27" t="s">
         <v>8</v>
       </c>
       <c r="F27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1209,13 +1209,13 @@
         <v>2</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E28" t="s">
         <v>8</v>
       </c>
       <c r="F28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1229,13 +1229,13 @@
         <v>1</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E29" t="s">
         <v>8</v>
       </c>
       <c r="F29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1249,13 +1249,13 @@
         <v>2</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E30" t="s">
         <v>8</v>
       </c>
       <c r="F30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1269,7 +1269,7 @@
         <v>1</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E31" t="s">
         <v>8</v>
@@ -1286,13 +1286,13 @@
         <v>2</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E32" t="s">
         <v>8</v>
       </c>
       <c r="F32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -1306,7 +1306,7 @@
         <v>1</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E33" t="s">
         <v>8</v>
@@ -1323,16 +1323,16 @@
         <v>2</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E34" t="s">
         <v>8</v>
       </c>
       <c r="F34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -1346,7 +1346,7 @@
         <v>1</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E35" t="s">
         <v>8</v>
@@ -1363,16 +1363,16 @@
         <v>2</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E36" t="s">
         <v>8</v>
       </c>
       <c r="F36" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -1386,13 +1386,13 @@
         <v>1</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E37" t="s">
         <v>8</v>
       </c>
       <c r="F37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -1406,13 +1406,13 @@
         <v>2</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E38" t="s">
         <v>8</v>
       </c>
       <c r="F38" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -1426,7 +1426,7 @@
         <v>1</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E39" t="s">
         <v>8</v>
@@ -1443,16 +1443,16 @@
         <v>2</v>
       </c>
       <c r="D40" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E40" t="s">
+        <v>8</v>
+      </c>
+      <c r="F40" t="s">
         <v>49</v>
       </c>
-      <c r="E40" t="s">
-        <v>8</v>
-      </c>
-      <c r="F40" t="s">
-        <v>50</v>
-      </c>
       <c r="G40" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -1466,7 +1466,7 @@
         <v>1</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E41" t="s">
         <v>8</v>
@@ -1483,13 +1483,13 @@
         <v>2</v>
       </c>
       <c r="D42" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E42" t="s">
+        <v>8</v>
+      </c>
+      <c r="F42" t="s">
         <v>51</v>
-      </c>
-      <c r="E42" t="s">
-        <v>8</v>
-      </c>
-      <c r="F42" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -1503,7 +1503,7 @@
         <v>1</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E43" t="s">
         <v>8</v>
@@ -1520,13 +1520,13 @@
         <v>2</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E44" t="s">
         <v>8</v>
       </c>
       <c r="F44" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -1540,7 +1540,7 @@
         <v>1</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E45" t="s">
         <v>8</v>
@@ -1557,13 +1557,13 @@
         <v>2</v>
       </c>
       <c r="D46" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E46" t="s">
+        <v>8</v>
+      </c>
+      <c r="F46" t="s">
         <v>54</v>
-      </c>
-      <c r="E46" t="s">
-        <v>8</v>
-      </c>
-      <c r="F46" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -1577,7 +1577,7 @@
         <v>1</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E47" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
rebuild with new schedule
</commit_message>
<xml_diff>
--- a/BB512_Schedule.xlsx
+++ b/BB512_Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jones/Dropbox/_SDU_Teaching/BB512/Course Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF752C49-B5B8-F14E-AF0A-3BF786774FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD7C5F7-7835-184E-A788-CE6AD9FE5459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15540" xr2:uid="{CCA45BD5-8A90-4848-8BF8-FC958BC91D48}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="84">
   <si>
     <t>Topic</t>
   </si>
@@ -281,7 +281,10 @@
     <t>Practice Exam</t>
   </si>
   <si>
-    <t>Guest lecture: James Cant, jellyfish/coral population dynamics</t>
+    <t>Guest lecture: James Cant, coral population dynamics</t>
+  </si>
+  <si>
+    <t>Guest lecture: Morgane Tidière, Sex differences in demography</t>
   </si>
 </sst>
 </file>
@@ -651,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C11A616-6116-174C-ABC2-888311E75E63}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1510,10 +1513,10 @@
         <v>18</v>
       </c>
       <c r="C43" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>26</v>
+        <v>83</v>
       </c>
       <c r="E43" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Updated schedule to add correct name to first practical.
</commit_message>
<xml_diff>
--- a/BB512_Schedule.xlsx
+++ b/BB512_Schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jones/Dropbox/_SDU_Teaching/BB512/BB512_Book/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jones/Dropbox/_SDU_Teaching/BB512/Course Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8276BDEF-6982-D54D-A7D4-6DC492390FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF0B398-86B6-8C44-81E9-30C8ADBCC22D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="31980" windowHeight="28120" xr2:uid="{CCA45BD5-8A90-4848-8BF8-FC958BC91D48}"/>
   </bookViews>
@@ -212,9 +212,6 @@
     <t>Exercises on game theory</t>
   </si>
   <si>
-    <t>Exercises on natural selection</t>
-  </si>
-  <si>
     <t>Exercise - Bug hunt camouflage (NetLogo)</t>
   </si>
   <si>
@@ -285,6 +282,9 @@
   </si>
   <si>
     <t xml:space="preserve">Exercises on Lotka-Volterra predator-prey dynamics (part 1) </t>
+  </si>
+  <si>
+    <t>Exercise - Randomness and Perfection</t>
   </si>
 </sst>
 </file>
@@ -823,7 +823,7 @@
   <dimension ref="A1:M51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="144" zoomScaleNormal="144" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -844,7 +844,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>4</v>
@@ -876,7 +876,7 @@
         <v>22</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>18</v>
@@ -897,7 +897,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="F3" s="10"/>
       <c r="G3" s="12" t="s">
@@ -942,7 +942,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F5" s="15"/>
       <c r="G5" s="17" t="s">
@@ -966,7 +966,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>14</v>
@@ -990,7 +990,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="12" t="s">
@@ -1012,7 +1012,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>15</v>
@@ -1035,7 +1035,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="12" t="s">
@@ -1079,7 +1079,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F11" s="10"/>
       <c r="G11" s="12" t="s">
@@ -1123,7 +1123,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="12" t="s">
@@ -1167,7 +1167,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F15" s="15"/>
       <c r="G15" s="17" t="s">
@@ -1213,7 +1213,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="12" t="s">
@@ -1257,7 +1257,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F19" s="10"/>
       <c r="G19" s="12" t="s">
@@ -1301,7 +1301,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F21" s="10"/>
       <c r="G21" s="12" t="s">
@@ -1343,7 +1343,7 @@
         <v>1</v>
       </c>
       <c r="E23" s="24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G23" s="22" t="s">
         <v>18</v>
@@ -1384,7 +1384,7 @@
         <v>1</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="12" t="s">
@@ -1427,7 +1427,7 @@
         <v>1</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F27" s="10"/>
       <c r="G27" s="12" t="s">
@@ -1472,7 +1472,7 @@
         <v>1</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F29" s="10"/>
       <c r="G29" s="12" t="s">
@@ -1495,7 +1495,7 @@
         <v>39</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G30" s="12" t="s">
         <v>18</v>
@@ -1647,7 +1647,7 @@
         <v>1</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F37" s="10"/>
       <c r="G37" s="12" t="s">
@@ -1759,7 +1759,7 @@
         <v>9</v>
       </c>
       <c r="F42" s="27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G42" s="28" t="s">
         <v>18</v>
@@ -1779,7 +1779,7 @@
         <v>1</v>
       </c>
       <c r="E43" s="24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F43" s="25"/>
       <c r="G43" s="22" t="s">
@@ -1803,7 +1803,7 @@
         <v>45</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G44" s="12" t="s">
         <v>18</v>
@@ -1848,7 +1848,7 @@
         <v>35</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G46" s="12" t="s">
         <v>18</v>
@@ -1868,7 +1868,7 @@
         <v>1</v>
       </c>
       <c r="E47" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F47" s="15"/>
       <c r="G47" s="17" t="s">
@@ -2017,7 +2017,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>